<commit_message>
Add anomalis and handling of it
</commit_message>
<xml_diff>
--- a/Data/gender_classification_data.xlsx
+++ b/Data/gender_classification_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simranraina\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF7E8A79-D68B-489C-B750-4130683BD230}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D04F99-037A-48E5-9AA2-C9C6970849F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7D811102-B255-41A8-97E2-E7EF1D627FE5}"/>
+    <workbookView xWindow="180" yWindow="0" windowWidth="19020" windowHeight="10200" xr2:uid="{7D811102-B255-41A8-97E2-E7EF1D627FE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="7">
   <si>
     <t>Height</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>Female</t>
+  </si>
+  <si>
+    <t>Height Inches</t>
   </si>
 </sst>
 </file>
@@ -411,20 +414,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D0A5C6A-2027-44F7-9288-992E10FBCD66}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:D44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="11.81640625" customWidth="1"/>
-    <col min="3" max="3" width="17.54296875" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="3" max="4" width="17.54296875" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -435,10 +438,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>180</v>
       </c>
@@ -448,11 +454,15 @@
       <c r="C2">
         <v>44</v>
       </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D2">
+        <f>A2*0.3937</f>
+        <v>70.866</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>178</v>
       </c>
@@ -462,11 +472,15 @@
       <c r="C3">
         <v>42</v>
       </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D3">
+        <f t="shared" ref="D3:D66" si="0">A3*0.3937</f>
+        <v>70.078599999999994</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>160</v>
       </c>
@@ -476,11 +490,15 @@
       <c r="C4">
         <v>38</v>
       </c>
-      <c r="D4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>62.991999999999997</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>140</v>
       </c>
@@ -490,25 +508,30 @@
       <c r="C5">
         <v>34</v>
       </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>55.118000000000002</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>130</v>
       </c>
       <c r="B6">
         <v>45</v>
       </c>
-      <c r="C6">
-        <v>32</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>51.180999999999997</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>144</v>
       </c>
@@ -518,11 +541,15 @@
       <c r="C7">
         <v>38</v>
       </c>
-      <c r="D7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>56.692799999999998</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>134</v>
       </c>
@@ -532,11 +559,15 @@
       <c r="C8">
         <v>36</v>
       </c>
-      <c r="D8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>52.755800000000001</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>188</v>
       </c>
@@ -546,11 +577,15 @@
       <c r="C9">
         <v>44</v>
       </c>
-      <c r="D9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>74.015599999999992</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>190</v>
       </c>
@@ -560,11 +595,15 @@
       <c r="C10">
         <v>44</v>
       </c>
-      <c r="D10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>74.802999999999997</v>
+      </c>
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>178</v>
       </c>
@@ -574,11 +613,15 @@
       <c r="C11">
         <v>42</v>
       </c>
-      <c r="D11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>70.078599999999994</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>172</v>
       </c>
@@ -588,11 +631,15 @@
       <c r="C12">
         <v>46</v>
       </c>
-      <c r="D12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>67.716399999999993</v>
+      </c>
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>164</v>
       </c>
@@ -602,11 +649,15 @@
       <c r="C13">
         <v>40</v>
       </c>
-      <c r="D13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>64.566800000000001</v>
+      </c>
+      <c r="E13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>154</v>
       </c>
@@ -616,11 +667,15 @@
       <c r="C14">
         <v>34</v>
       </c>
-      <c r="D14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>60.629799999999996</v>
+      </c>
+      <c r="E14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>168</v>
       </c>
@@ -630,25 +685,30 @@
       <c r="C15">
         <v>40</v>
       </c>
-      <c r="D15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>66.141599999999997</v>
+      </c>
+      <c r="E15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>146</v>
       </c>
-      <c r="B16">
-        <v>50</v>
-      </c>
       <c r="C16">
         <v>32</v>
       </c>
-      <c r="D16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>57.480199999999996</v>
+      </c>
+      <c r="E16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>180</v>
       </c>
@@ -658,11 +718,15 @@
       <c r="C17">
         <v>42</v>
       </c>
-      <c r="D17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>70.866</v>
+      </c>
+      <c r="E17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>182</v>
       </c>
@@ -672,11 +736,15 @@
       <c r="C18">
         <v>44</v>
       </c>
-      <c r="D18" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>71.653400000000005</v>
+      </c>
+      <c r="E18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>110</v>
       </c>
@@ -686,25 +754,30 @@
       <c r="C19">
         <v>38</v>
       </c>
-      <c r="D19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>43.307000000000002</v>
+      </c>
+      <c r="E19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>180</v>
       </c>
       <c r="B20">
         <v>78</v>
       </c>
-      <c r="C20">
-        <v>42</v>
-      </c>
-      <c r="D20" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>70.866</v>
+      </c>
+      <c r="E20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>146</v>
       </c>
@@ -714,11 +787,15 @@
       <c r="C21">
         <v>32</v>
       </c>
-      <c r="D21" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>57.480199999999996</v>
+      </c>
+      <c r="E21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>180</v>
       </c>
@@ -728,11 +805,15 @@
       <c r="C22">
         <v>42</v>
       </c>
-      <c r="D22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>70.866</v>
+      </c>
+      <c r="E22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>182</v>
       </c>
@@ -742,11 +823,15 @@
       <c r="C23">
         <v>44</v>
       </c>
-      <c r="D23" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>71.653400000000005</v>
+      </c>
+      <c r="E23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>134</v>
       </c>
@@ -756,11 +841,15 @@
       <c r="C24">
         <v>36</v>
       </c>
-      <c r="D24" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>52.755800000000001</v>
+      </c>
+      <c r="E24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>188</v>
       </c>
@@ -770,11 +859,15 @@
       <c r="C25">
         <v>44</v>
       </c>
-      <c r="D25" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>74.015599999999992</v>
+      </c>
+      <c r="E25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>190</v>
       </c>
@@ -784,11 +877,15 @@
       <c r="C26">
         <v>44</v>
       </c>
-      <c r="D26" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>74.802999999999997</v>
+      </c>
+      <c r="E26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>178</v>
       </c>
@@ -798,11 +895,15 @@
       <c r="C27">
         <v>42</v>
       </c>
-      <c r="D27" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>70.078599999999994</v>
+      </c>
+      <c r="E27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>172</v>
       </c>
@@ -812,11 +913,15 @@
       <c r="C28">
         <v>46</v>
       </c>
-      <c r="D28" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>67.716399999999993</v>
+      </c>
+      <c r="E28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>110</v>
       </c>
@@ -826,11 +931,15 @@
       <c r="C29">
         <v>38</v>
       </c>
-      <c r="D29" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>43.307000000000002</v>
+      </c>
+      <c r="E29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>180</v>
       </c>
@@ -840,11 +949,15 @@
       <c r="C30">
         <v>42</v>
       </c>
-      <c r="D30" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>70.866</v>
+      </c>
+      <c r="E30" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>146</v>
       </c>
@@ -854,11 +967,15 @@
       <c r="C31">
         <v>32</v>
       </c>
-      <c r="D31" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>57.480199999999996</v>
+      </c>
+      <c r="E31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>180</v>
       </c>
@@ -868,11 +985,15 @@
       <c r="C32">
         <v>42</v>
       </c>
-      <c r="D32" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>70.866</v>
+      </c>
+      <c r="E32" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>182</v>
       </c>
@@ -882,11 +1003,15 @@
       <c r="C33">
         <v>44</v>
       </c>
-      <c r="D33" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>71.653400000000005</v>
+      </c>
+      <c r="E33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>134</v>
       </c>
@@ -896,11 +1021,15 @@
       <c r="C34">
         <v>36</v>
       </c>
-      <c r="D34" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>52.755800000000001</v>
+      </c>
+      <c r="E34" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>188</v>
       </c>
@@ -910,11 +1039,15 @@
       <c r="C35">
         <v>44</v>
       </c>
-      <c r="D35" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>74.015599999999992</v>
+      </c>
+      <c r="E35" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>134</v>
       </c>
@@ -924,11 +1057,15 @@
       <c r="C36">
         <v>36</v>
       </c>
-      <c r="D36" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D36">
+        <f t="shared" si="0"/>
+        <v>52.755800000000001</v>
+      </c>
+      <c r="E36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>188</v>
       </c>
@@ -938,11 +1075,15 @@
       <c r="C37">
         <v>44</v>
       </c>
-      <c r="D37" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D37">
+        <f t="shared" si="0"/>
+        <v>74.015599999999992</v>
+      </c>
+      <c r="E37" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>190</v>
       </c>
@@ -952,25 +1093,30 @@
       <c r="C38">
         <v>44</v>
       </c>
-      <c r="D38" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D38">
+        <f t="shared" si="0"/>
+        <v>74.802999999999997</v>
+      </c>
+      <c r="E38" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>178</v>
       </c>
-      <c r="B39">
-        <v>78</v>
-      </c>
       <c r="C39">
         <v>42</v>
       </c>
-      <c r="D39" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D39">
+        <f t="shared" si="0"/>
+        <v>70.078599999999994</v>
+      </c>
+      <c r="E39" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>182</v>
       </c>
@@ -980,11 +1126,15 @@
       <c r="C40">
         <v>44</v>
       </c>
-      <c r="D40" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D40">
+        <f t="shared" si="0"/>
+        <v>71.653400000000005</v>
+      </c>
+      <c r="E40" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>134</v>
       </c>
@@ -994,8 +1144,1092 @@
       <c r="C41">
         <v>36</v>
       </c>
-      <c r="D41" t="s">
-        <v>5</v>
+      <c r="D41">
+        <f t="shared" si="0"/>
+        <v>52.755800000000001</v>
+      </c>
+      <c r="E41" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>188</v>
+      </c>
+      <c r="B42">
+        <v>84</v>
+      </c>
+      <c r="C42">
+        <v>44</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="0"/>
+        <v>74.015599999999992</v>
+      </c>
+      <c r="E42" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>190</v>
+      </c>
+      <c r="B43">
+        <v>88</v>
+      </c>
+      <c r="C43">
+        <v>44</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="0"/>
+        <v>74.802999999999997</v>
+      </c>
+      <c r="E43" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>178</v>
+      </c>
+      <c r="B44">
+        <v>78</v>
+      </c>
+      <c r="C44">
+        <v>42</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="0"/>
+        <v>70.078599999999994</v>
+      </c>
+      <c r="E44" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>172</v>
+      </c>
+      <c r="B45">
+        <v>74</v>
+      </c>
+      <c r="C45">
+        <v>46</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="0"/>
+        <v>67.716399999999993</v>
+      </c>
+      <c r="E45" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>110</v>
+      </c>
+      <c r="B46">
+        <v>50</v>
+      </c>
+      <c r="C46">
+        <v>38</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="0"/>
+        <v>43.307000000000002</v>
+      </c>
+      <c r="E46" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>180</v>
+      </c>
+      <c r="B47">
+        <v>78</v>
+      </c>
+      <c r="C47">
+        <v>42</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="0"/>
+        <v>70.866</v>
+      </c>
+      <c r="E47" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>146</v>
+      </c>
+      <c r="B48">
+        <v>50</v>
+      </c>
+      <c r="C48">
+        <v>32</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="0"/>
+        <v>57.480199999999996</v>
+      </c>
+      <c r="E48" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>180</v>
+      </c>
+      <c r="B49">
+        <v>82</v>
+      </c>
+      <c r="C49">
+        <v>42</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="0"/>
+        <v>70.866</v>
+      </c>
+      <c r="E49" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>182</v>
+      </c>
+      <c r="B50">
+        <v>84</v>
+      </c>
+      <c r="C50">
+        <v>44</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="0"/>
+        <v>71.653400000000005</v>
+      </c>
+      <c r="E50" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>134</v>
+      </c>
+      <c r="B51">
+        <v>52</v>
+      </c>
+      <c r="C51">
+        <v>36</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="0"/>
+        <v>52.755800000000001</v>
+      </c>
+      <c r="E51" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>188</v>
+      </c>
+      <c r="B52">
+        <v>84</v>
+      </c>
+      <c r="C52">
+        <v>44</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="0"/>
+        <v>74.015599999999992</v>
+      </c>
+      <c r="E52" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>134</v>
+      </c>
+      <c r="B53">
+        <v>52</v>
+      </c>
+      <c r="C53">
+        <v>36</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="0"/>
+        <v>52.755800000000001</v>
+      </c>
+      <c r="E53" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>188</v>
+      </c>
+      <c r="B54">
+        <v>84</v>
+      </c>
+      <c r="C54">
+        <v>44</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="0"/>
+        <v>74.015599999999992</v>
+      </c>
+      <c r="E54" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>190</v>
+      </c>
+      <c r="B55">
+        <v>88</v>
+      </c>
+      <c r="C55">
+        <v>44</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="0"/>
+        <v>74.802999999999997</v>
+      </c>
+      <c r="E55" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>110</v>
+      </c>
+      <c r="B56">
+        <v>50</v>
+      </c>
+      <c r="C56">
+        <v>38</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="0"/>
+        <v>43.307000000000002</v>
+      </c>
+      <c r="E56" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>180</v>
+      </c>
+      <c r="B57">
+        <v>78</v>
+      </c>
+      <c r="C57">
+        <v>42</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="0"/>
+        <v>70.866</v>
+      </c>
+      <c r="E57" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <v>146</v>
+      </c>
+      <c r="B58">
+        <v>50</v>
+      </c>
+      <c r="C58">
+        <v>32</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="0"/>
+        <v>57.480199999999996</v>
+      </c>
+      <c r="E58" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>180</v>
+      </c>
+      <c r="B59">
+        <v>82</v>
+      </c>
+      <c r="C59">
+        <v>42</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="0"/>
+        <v>70.866</v>
+      </c>
+      <c r="E59" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>182</v>
+      </c>
+      <c r="B60">
+        <v>84</v>
+      </c>
+      <c r="C60">
+        <v>44</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="0"/>
+        <v>71.653400000000005</v>
+      </c>
+      <c r="E60" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <v>182</v>
+      </c>
+      <c r="B61">
+        <v>84</v>
+      </c>
+      <c r="C61">
+        <v>44</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="0"/>
+        <v>71.653400000000005</v>
+      </c>
+      <c r="E61" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <v>134</v>
+      </c>
+      <c r="B62">
+        <v>52</v>
+      </c>
+      <c r="C62">
+        <v>36</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="0"/>
+        <v>52.755800000000001</v>
+      </c>
+      <c r="E62" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A63">
+        <v>188</v>
+      </c>
+      <c r="B63">
+        <v>84</v>
+      </c>
+      <c r="C63">
+        <v>44</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="0"/>
+        <v>74.015599999999992</v>
+      </c>
+      <c r="E63" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A64">
+        <v>110</v>
+      </c>
+      <c r="B64">
+        <v>50</v>
+      </c>
+      <c r="C64">
+        <v>38</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="0"/>
+        <v>43.307000000000002</v>
+      </c>
+      <c r="E64" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A65">
+        <v>180</v>
+      </c>
+      <c r="B65">
+        <v>78</v>
+      </c>
+      <c r="C65">
+        <v>42</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="0"/>
+        <v>70.866</v>
+      </c>
+      <c r="E65" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A66">
+        <v>146</v>
+      </c>
+      <c r="B66">
+        <v>50</v>
+      </c>
+      <c r="C66">
+        <v>32</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="0"/>
+        <v>57.480199999999996</v>
+      </c>
+      <c r="E66" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A67">
+        <v>180</v>
+      </c>
+      <c r="B67">
+        <v>82</v>
+      </c>
+      <c r="C67">
+        <v>42</v>
+      </c>
+      <c r="D67">
+        <f t="shared" ref="D67:D101" si="1">A67*0.3937</f>
+        <v>70.866</v>
+      </c>
+      <c r="E67" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A68">
+        <v>182</v>
+      </c>
+      <c r="B68">
+        <v>84</v>
+      </c>
+      <c r="C68">
+        <v>44</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="1"/>
+        <v>71.653400000000005</v>
+      </c>
+      <c r="E68" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A69">
+        <v>134</v>
+      </c>
+      <c r="B69">
+        <v>52</v>
+      </c>
+      <c r="C69">
+        <v>36</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="1"/>
+        <v>52.755800000000001</v>
+      </c>
+      <c r="E69" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A70">
+        <v>188</v>
+      </c>
+      <c r="B70">
+        <v>84</v>
+      </c>
+      <c r="C70">
+        <v>44</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="1"/>
+        <v>74.015599999999992</v>
+      </c>
+      <c r="E70" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A71">
+        <v>134</v>
+      </c>
+      <c r="B71">
+        <v>52</v>
+      </c>
+      <c r="C71">
+        <v>36</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="1"/>
+        <v>52.755800000000001</v>
+      </c>
+      <c r="E71" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A72">
+        <v>188</v>
+      </c>
+      <c r="B72">
+        <v>84</v>
+      </c>
+      <c r="C72">
+        <v>44</v>
+      </c>
+      <c r="D72">
+        <f t="shared" si="1"/>
+        <v>74.015599999999992</v>
+      </c>
+      <c r="E72" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A73">
+        <v>134</v>
+      </c>
+      <c r="B73">
+        <v>52</v>
+      </c>
+      <c r="C73">
+        <v>36</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="1"/>
+        <v>52.755800000000001</v>
+      </c>
+      <c r="E73" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A74">
+        <v>100</v>
+      </c>
+      <c r="B74">
+        <v>30</v>
+      </c>
+      <c r="C74">
+        <v>30</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="1"/>
+        <v>39.369999999999997</v>
+      </c>
+      <c r="E74" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A75">
+        <v>220</v>
+      </c>
+      <c r="B75">
+        <v>140</v>
+      </c>
+      <c r="C75">
+        <v>50</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="1"/>
+        <v>86.614000000000004</v>
+      </c>
+      <c r="E75" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A76">
+        <v>182</v>
+      </c>
+      <c r="B76">
+        <v>84</v>
+      </c>
+      <c r="C76">
+        <v>44</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="1"/>
+        <v>71.653400000000005</v>
+      </c>
+      <c r="E76" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A77">
+        <v>134</v>
+      </c>
+      <c r="B77">
+        <v>52</v>
+      </c>
+      <c r="C77">
+        <v>36</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="1"/>
+        <v>52.755800000000001</v>
+      </c>
+      <c r="E77" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A78">
+        <v>188</v>
+      </c>
+      <c r="B78">
+        <v>84</v>
+      </c>
+      <c r="C78">
+        <v>44</v>
+      </c>
+      <c r="D78">
+        <f t="shared" si="1"/>
+        <v>74.015599999999992</v>
+      </c>
+      <c r="E78" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A79">
+        <v>190</v>
+      </c>
+      <c r="B79">
+        <v>88</v>
+      </c>
+      <c r="C79">
+        <v>44</v>
+      </c>
+      <c r="D79">
+        <f t="shared" si="1"/>
+        <v>74.802999999999997</v>
+      </c>
+      <c r="E79" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A80">
+        <v>178</v>
+      </c>
+      <c r="B80">
+        <v>78</v>
+      </c>
+      <c r="C80">
+        <v>42</v>
+      </c>
+      <c r="D80">
+        <f t="shared" si="1"/>
+        <v>70.078599999999994</v>
+      </c>
+      <c r="E80" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A81">
+        <v>172</v>
+      </c>
+      <c r="B81">
+        <v>74</v>
+      </c>
+      <c r="C81">
+        <v>46</v>
+      </c>
+      <c r="D81">
+        <f t="shared" si="1"/>
+        <v>67.716399999999993</v>
+      </c>
+      <c r="E81" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A82">
+        <v>110</v>
+      </c>
+      <c r="B82">
+        <v>50</v>
+      </c>
+      <c r="C82">
+        <v>38</v>
+      </c>
+      <c r="D82">
+        <f t="shared" si="1"/>
+        <v>43.307000000000002</v>
+      </c>
+      <c r="E82" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A83">
+        <v>134</v>
+      </c>
+      <c r="B83">
+        <v>52</v>
+      </c>
+      <c r="C83">
+        <v>36</v>
+      </c>
+      <c r="D83">
+        <f t="shared" si="1"/>
+        <v>52.755800000000001</v>
+      </c>
+      <c r="E83" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A84">
+        <v>188</v>
+      </c>
+      <c r="B84">
+        <v>84</v>
+      </c>
+      <c r="C84">
+        <v>44</v>
+      </c>
+      <c r="D84">
+        <f t="shared" si="1"/>
+        <v>74.015599999999992</v>
+      </c>
+      <c r="E84" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A85">
+        <v>190</v>
+      </c>
+      <c r="B85">
+        <v>88</v>
+      </c>
+      <c r="C85">
+        <v>44</v>
+      </c>
+      <c r="D85">
+        <f t="shared" si="1"/>
+        <v>74.802999999999997</v>
+      </c>
+      <c r="E85" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A86">
+        <v>178</v>
+      </c>
+      <c r="B86">
+        <v>78</v>
+      </c>
+      <c r="C86">
+        <v>42</v>
+      </c>
+      <c r="D86">
+        <f t="shared" si="1"/>
+        <v>70.078599999999994</v>
+      </c>
+      <c r="E86" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A87">
+        <v>172</v>
+      </c>
+      <c r="B87">
+        <v>74</v>
+      </c>
+      <c r="C87">
+        <v>46</v>
+      </c>
+      <c r="D87">
+        <f t="shared" si="1"/>
+        <v>67.716399999999993</v>
+      </c>
+      <c r="E87" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A88">
+        <v>134</v>
+      </c>
+      <c r="B88">
+        <v>52</v>
+      </c>
+      <c r="C88">
+        <v>36</v>
+      </c>
+      <c r="D88">
+        <f t="shared" si="1"/>
+        <v>52.755800000000001</v>
+      </c>
+      <c r="E88" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A89">
+        <v>188</v>
+      </c>
+      <c r="B89">
+        <v>84</v>
+      </c>
+      <c r="C89">
+        <v>44</v>
+      </c>
+      <c r="D89">
+        <f t="shared" si="1"/>
+        <v>74.015599999999992</v>
+      </c>
+      <c r="E89" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A90">
+        <v>190</v>
+      </c>
+      <c r="B90">
+        <v>88</v>
+      </c>
+      <c r="C90">
+        <v>44</v>
+      </c>
+      <c r="D90">
+        <f t="shared" si="1"/>
+        <v>74.802999999999997</v>
+      </c>
+      <c r="E90" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A91">
+        <v>180</v>
+      </c>
+      <c r="B91">
+        <v>80</v>
+      </c>
+      <c r="C91">
+        <v>44</v>
+      </c>
+      <c r="D91">
+        <f t="shared" si="1"/>
+        <v>70.866</v>
+      </c>
+      <c r="E91" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A92">
+        <v>178</v>
+      </c>
+      <c r="B92">
+        <v>78</v>
+      </c>
+      <c r="C92">
+        <v>42</v>
+      </c>
+      <c r="D92">
+        <f t="shared" si="1"/>
+        <v>70.078599999999994</v>
+      </c>
+      <c r="E92" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A93">
+        <v>160</v>
+      </c>
+      <c r="B93">
+        <v>60</v>
+      </c>
+      <c r="C93">
+        <v>38</v>
+      </c>
+      <c r="D93">
+        <f t="shared" si="1"/>
+        <v>62.991999999999997</v>
+      </c>
+      <c r="E93" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A94">
+        <v>140</v>
+      </c>
+      <c r="B94">
+        <v>50</v>
+      </c>
+      <c r="C94">
+        <v>34</v>
+      </c>
+      <c r="D94">
+        <f t="shared" si="1"/>
+        <v>55.118000000000002</v>
+      </c>
+      <c r="E94" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A95">
+        <v>180</v>
+      </c>
+      <c r="B95">
+        <v>82</v>
+      </c>
+      <c r="C95">
+        <v>42</v>
+      </c>
+      <c r="D95">
+        <f t="shared" si="1"/>
+        <v>70.866</v>
+      </c>
+      <c r="E95" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A96">
+        <v>182</v>
+      </c>
+      <c r="B96">
+        <v>84</v>
+      </c>
+      <c r="C96">
+        <v>44</v>
+      </c>
+      <c r="D96">
+        <f t="shared" si="1"/>
+        <v>71.653400000000005</v>
+      </c>
+      <c r="E96" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A97">
+        <v>134</v>
+      </c>
+      <c r="B97">
+        <v>52</v>
+      </c>
+      <c r="C97">
+        <v>36</v>
+      </c>
+      <c r="D97">
+        <f t="shared" si="1"/>
+        <v>52.755800000000001</v>
+      </c>
+      <c r="E97" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A98">
+        <v>188</v>
+      </c>
+      <c r="B98">
+        <v>84</v>
+      </c>
+      <c r="C98">
+        <v>44</v>
+      </c>
+      <c r="D98">
+        <f t="shared" si="1"/>
+        <v>74.015599999999992</v>
+      </c>
+      <c r="E98" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A99">
+        <v>134</v>
+      </c>
+      <c r="B99">
+        <v>52</v>
+      </c>
+      <c r="C99">
+        <v>36</v>
+      </c>
+      <c r="D99">
+        <f t="shared" si="1"/>
+        <v>52.755800000000001</v>
+      </c>
+      <c r="E99" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A100">
+        <v>188</v>
+      </c>
+      <c r="B100">
+        <v>84</v>
+      </c>
+      <c r="C100">
+        <v>44</v>
+      </c>
+      <c r="D100">
+        <f t="shared" si="1"/>
+        <v>74.015599999999992</v>
+      </c>
+      <c r="E100" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A101">
+        <v>178</v>
+      </c>
+      <c r="B101">
+        <v>78</v>
+      </c>
+      <c r="C101">
+        <v>42</v>
+      </c>
+      <c r="D101">
+        <f t="shared" si="1"/>
+        <v>70.078599999999994</v>
+      </c>
+      <c r="E101" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>